<commit_message>
LAPR5 - Avaliação Pares [ref issue #47]
</commit_message>
<xml_diff>
--- a/taskslapr5.xlsx
+++ b/taskslapr5.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carlosmoreira/OneDrive/OneDrive - Instituto Superior de Engenharia do Porto/ISEP/3A/LAPR5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90421375-6FBA-3C4D-9398-9A24D144D6EF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0341F6B-5A9F-554F-BCC0-1319E3AAD9E0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35940" yWindow="-520" windowWidth="33600" windowHeight="19480" xr2:uid="{30B2DF19-576D-0644-861A-5EEAB883D1E5}"/>
+    <workbookView xWindow="1020" yWindow="2960" windowWidth="30200" windowHeight="14820" activeTab="2" xr2:uid="{30B2DF19-576D-0644-861A-5EEAB883D1E5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint1" sheetId="2" r:id="rId1"/>
     <sheet name="Sprint2" sheetId="3" r:id="rId2"/>
+    <sheet name="Sprint3" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="134">
   <si>
     <t>Criar Produto, definindo o plano de fabrico</t>
   </si>
@@ -368,13 +369,93 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>sprint</t>
+  </si>
+  <si>
+    <t>módulo</t>
+  </si>
+  <si>
+    <t>requisito</t>
+  </si>
+  <si>
+    <t>descrição breve/user story</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>- introduzir o conceito de produto, com várias operações, e de linha de produção, com várias máquinas, com vista ao escalonamento de produtos numa linha de produção</t>
+  </si>
+  <si>
+    <t>-  introduzir o conceito de cliente, com prioridades, e de encomendas de várias unidades de vários produtos</t>
+  </si>
+  <si>
+    <t>- aplicar um método de pesquisa automática (Algoritmos Genéticos ou outro) e gerar soluções que minimizem: soma de atrasos das encomendas; nº de encomendas atrasadas; nº de clientes com atraso; impacto nos clientes de acordo com as suas prioridades</t>
+  </si>
+  <si>
+    <t>Serviço Gestão de Encomendas em node.js
+- Criar Cliente
+- Criar Encomenda
+- Alterar Cliente (nome, endereço)
+- Alterar Encomenda
+- Cancelar Encomenda
+- Consultar Cliente
+- Consultar Encomenda</t>
+  </si>
+  <si>
+    <t>UI Gestão de Encomendas na SPA existente
+- Criar Cliente
+- Criar Encomenda
+- Alterar Cliente (nome, endereço)
+- Alterar Encomenda
+- Cancelar Encomenda
+- Consultar Cliente
+- Consultar Encomenda</t>
+  </si>
+  <si>
+    <t>implantação de serviços GE, MDF, MDP em máquina virtual, contentores ou nuvem (pelo menos um dos serviços nas MV de ASIST)</t>
+  </si>
+  <si>
+    <t>Autentição e autorização na SPA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Como administrador da infraestrutura quero que seja criada uma SAN iSCSI nos servidores Linux e Windows disponíveis para qualquer utilizador autenticado </t>
+  </si>
+  <si>
+    <t>Como administrador da infraestrutura quero que a SAN anterior esteja disponível sem necessidade de intervenção humana após um reboot de qualquer dos servidores</t>
+  </si>
+  <si>
+    <t>Como administrador do servidor Linux quero que semanalmente seja verificado se todos os utilizadores registados em /etc/passwd possuem uma entrada no /etc/shadow, se o grupo primário existe, se a homedir existe e pertence ao dono e grupo correto. Qualquer inconformidade deve ser registada em /tmp/auth_error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Como administrador da infraestrutura quero que todos os utilizadores registados no DC Windows tenham a sessão bloqueada ao fim de 1 minuto de inatividade </t>
+  </si>
+  <si>
+    <t>Gestão de encomendas</t>
+  </si>
+  <si>
+    <t>registo de utilizadores com informação da politica de privacidade e recolha de consentimentos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implementar a opção que permita o exercício do direito ao esquecimento (RGPD) no módulo de Gestão de Encomendas </t>
+  </si>
+  <si>
+    <t>Edição de chão de fábrica com o recurso aos widgets. A representação gráfica deverá reflectir as alterações efectuadas nos widgets.</t>
+  </si>
+  <si>
+    <t>Feedback para o utilizador: apresentação de tooltips contendo informação acerca das características do objecto (máquina, produto) apontado pelo cursor gráfico; consequente remoção do tooltip quando o cursor é afastado do objecto.</t>
+  </si>
+  <si>
+    <t>Animação do plano de produção.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -417,8 +498,36 @@
       <name val="Helvetica"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -461,8 +570,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF4472C4"/>
+        <bgColor rgb="FF4472C4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9E1F2"/>
+        <bgColor rgb="FFD9E1F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -570,11 +697,120 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF8EA9DB"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF8EA9DB"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF8EA9DB"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF8EA9DB"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF8EA9DB"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF8EA9DB"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF8EA9DB"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF8EA9DB"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF8EA9DB"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF8EA9DB"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF8EA9DB"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF8EA9DB"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF8EA9DB"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF8EA9DB"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF8EA9DB"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF8EA9DB"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF8EA9DB"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF8EA9DB"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -648,6 +884,9 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -665,6 +904,37 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -982,7 +1252,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A371274-109E-C842-A589-0EE61A75A451}">
   <dimension ref="B1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+    <sheetView zoomScale="125" workbookViewId="0">
       <selection activeCell="C18" sqref="C18:G18"/>
     </sheetView>
   </sheetViews>
@@ -1003,7 +1273,7 @@
       <c r="H2" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="J2" s="28" t="s">
+      <c r="J2" s="29" t="s">
         <v>110</v>
       </c>
     </row>
@@ -1011,20 +1281,20 @@
       <c r="B3" s="11">
         <v>1</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
       <c r="H3" s="12">
         <v>40</v>
       </c>
       <c r="I3" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="J3" s="29"/>
+      <c r="J3" s="30"/>
       <c r="K3" s="14" t="s">
         <v>57</v>
       </c>
@@ -1036,13 +1306,13 @@
       <c r="B4" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
       <c r="H4" s="7">
         <v>4</v>
       </c>
@@ -1061,13 +1331,13 @@
       <c r="B5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="27"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="28"/>
       <c r="H5" s="7">
         <v>4</v>
       </c>
@@ -1086,13 +1356,13 @@
       <c r="B6" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="27" t="s">
+      <c r="C6" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
       <c r="H6" s="7">
         <v>4</v>
       </c>
@@ -1111,13 +1381,13 @@
       <c r="B7" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="27" t="s">
+      <c r="C7" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
       <c r="H7" s="7">
         <v>2</v>
       </c>
@@ -1136,13 +1406,13 @@
       <c r="B8" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="27" t="s">
+      <c r="C8" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="27"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
       <c r="H8" s="7">
         <v>4</v>
       </c>
@@ -1161,13 +1431,13 @@
       <c r="B9" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="27" t="s">
+      <c r="C9" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
       <c r="H9" s="7">
         <v>4</v>
       </c>
@@ -1186,13 +1456,13 @@
       <c r="B10" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="27" t="s">
+      <c r="C10" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
       <c r="H10" s="7">
         <v>4</v>
       </c>
@@ -1211,13 +1481,13 @@
       <c r="B11" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="27" t="s">
+      <c r="C11" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="27"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
       <c r="H11" s="7">
         <v>2</v>
       </c>
@@ -1236,13 +1506,13 @@
       <c r="B12" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="27" t="s">
+      <c r="C12" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="28"/>
       <c r="H12" s="7">
         <v>2</v>
       </c>
@@ -1261,13 +1531,13 @@
       <c r="B13" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="27" t="s">
+      <c r="C13" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="27"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="27"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="28"/>
       <c r="H13" s="7">
         <v>2</v>
       </c>
@@ -1286,13 +1556,13 @@
       <c r="B14" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="27" t="s">
+      <c r="C14" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
       <c r="H14" s="7">
         <v>2</v>
       </c>
@@ -1311,13 +1581,13 @@
       <c r="B15" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="27" t="s">
+      <c r="C15" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="D15" s="27"/>
-      <c r="E15" s="27"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="27"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="28"/>
       <c r="H15" s="7">
         <v>2</v>
       </c>
@@ -1336,13 +1606,13 @@
       <c r="B16" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="25" t="s">
+      <c r="C16" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="25"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="26"/>
       <c r="H16" s="8">
         <v>4</v>
       </c>
@@ -1361,13 +1631,13 @@
       <c r="B17" s="11">
         <v>2</v>
       </c>
-      <c r="C17" s="26" t="s">
+      <c r="C17" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="D17" s="26"/>
-      <c r="E17" s="26"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="26"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="27"/>
       <c r="H17" s="12">
         <v>25</v>
       </c>
@@ -1376,13 +1646,13 @@
       <c r="B18" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="27" t="s">
+      <c r="C18" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="D18" s="27"/>
-      <c r="E18" s="27"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="27"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="28"/>
       <c r="H18" s="7">
         <v>-20</v>
       </c>
@@ -1394,13 +1664,13 @@
       <c r="B19" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="27" t="s">
+      <c r="C19" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="D19" s="27"/>
-      <c r="E19" s="27"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="27"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="28"/>
+      <c r="G19" s="28"/>
       <c r="H19" s="7">
         <v>-5</v>
       </c>
@@ -1412,13 +1682,13 @@
       <c r="B20" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="27" t="s">
+      <c r="C20" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="D20" s="27"/>
-      <c r="E20" s="27"/>
-      <c r="F20" s="27"/>
-      <c r="G20" s="27"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="28"/>
       <c r="H20" s="7">
         <v>5</v>
       </c>
@@ -1430,13 +1700,13 @@
       <c r="B21" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="27" t="s">
+      <c r="C21" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="D21" s="27"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="27"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="28"/>
+      <c r="G21" s="28"/>
       <c r="H21" s="7">
         <v>10</v>
       </c>
@@ -1448,13 +1718,13 @@
       <c r="B22" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C22" s="27" t="s">
+      <c r="C22" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="D22" s="27"/>
-      <c r="E22" s="27"/>
-      <c r="F22" s="27"/>
-      <c r="G22" s="27"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="28"/>
+      <c r="F22" s="28"/>
+      <c r="G22" s="28"/>
       <c r="H22" s="7">
         <v>5</v>
       </c>
@@ -1466,13 +1736,13 @@
       <c r="B23" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C23" s="27" t="s">
+      <c r="C23" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="D23" s="27"/>
-      <c r="E23" s="27"/>
-      <c r="F23" s="27"/>
-      <c r="G23" s="27"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="28"/>
+      <c r="G23" s="28"/>
       <c r="H23" s="7">
         <v>5</v>
       </c>
@@ -1484,13 +1754,13 @@
       <c r="B24" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C24" s="25" t="s">
+      <c r="C24" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="D24" s="25"/>
-      <c r="E24" s="25"/>
-      <c r="F24" s="25"/>
-      <c r="G24" s="25"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="26"/>
       <c r="H24" s="8">
         <v>-10</v>
       </c>
@@ -1499,13 +1769,13 @@
       <c r="B25" s="11">
         <v>3</v>
       </c>
-      <c r="C25" s="26" t="s">
+      <c r="C25" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="D25" s="26"/>
-      <c r="E25" s="26"/>
-      <c r="F25" s="26"/>
-      <c r="G25" s="26"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="27"/>
+      <c r="F25" s="27"/>
+      <c r="G25" s="27"/>
       <c r="H25" s="12">
         <v>30</v>
       </c>
@@ -1514,13 +1784,13 @@
       <c r="B26" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="C26" s="27" t="s">
+      <c r="C26" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="D26" s="27"/>
-      <c r="E26" s="27"/>
-      <c r="F26" s="27"/>
-      <c r="G26" s="27"/>
+      <c r="D26" s="28"/>
+      <c r="E26" s="28"/>
+      <c r="F26" s="28"/>
+      <c r="G26" s="28"/>
       <c r="H26" s="7">
         <v>10</v>
       </c>
@@ -1532,13 +1802,13 @@
       <c r="B27" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="27" t="s">
+      <c r="C27" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="D27" s="27"/>
-      <c r="E27" s="27"/>
-      <c r="F27" s="27"/>
-      <c r="G27" s="27"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="28"/>
+      <c r="F27" s="28"/>
+      <c r="G27" s="28"/>
       <c r="H27" s="7">
         <v>20</v>
       </c>
@@ -1550,13 +1820,13 @@
       <c r="B28" s="11">
         <v>4</v>
       </c>
-      <c r="C28" s="26" t="s">
+      <c r="C28" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="D28" s="26"/>
-      <c r="E28" s="26"/>
-      <c r="F28" s="26"/>
-      <c r="G28" s="26"/>
+      <c r="D28" s="27"/>
+      <c r="E28" s="27"/>
+      <c r="F28" s="27"/>
+      <c r="G28" s="27"/>
       <c r="H28" s="12">
         <v>25</v>
       </c>
@@ -1565,13 +1835,13 @@
       <c r="B29" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C29" s="27" t="s">
+      <c r="C29" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
+      <c r="D29" s="28"/>
+      <c r="E29" s="28"/>
+      <c r="F29" s="28"/>
+      <c r="G29" s="28"/>
       <c r="H29" s="7">
         <v>5</v>
       </c>
@@ -1580,13 +1850,13 @@
       <c r="B30" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="C30" s="27" t="s">
+      <c r="C30" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
+      <c r="D30" s="28"/>
+      <c r="E30" s="28"/>
+      <c r="F30" s="28"/>
+      <c r="G30" s="28"/>
       <c r="H30" s="7">
         <v>10</v>
       </c>
@@ -1595,13 +1865,13 @@
       <c r="B31" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="C31" s="25" t="s">
+      <c r="C31" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="D31" s="25"/>
-      <c r="E31" s="25"/>
-      <c r="F31" s="25"/>
-      <c r="G31" s="25"/>
+      <c r="D31" s="26"/>
+      <c r="E31" s="26"/>
+      <c r="F31" s="26"/>
+      <c r="G31" s="26"/>
       <c r="H31" s="8">
         <v>10</v>
       </c>
@@ -1648,8 +1918,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82610D93-8C3C-8245-A778-8DFEFA3C3A6C}">
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1732,13 +2002,13 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="30" t="s">
+      <c r="A6" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="C6" s="30">
+      <c r="C6" s="31">
         <v>5</v>
       </c>
       <c r="D6" s="17" t="s">
@@ -1746,93 +2016,93 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="30"/>
-      <c r="B7" s="30"/>
-      <c r="C7" s="30"/>
+      <c r="A7" s="31"/>
+      <c r="B7" s="31"/>
+      <c r="C7" s="31"/>
       <c r="D7" s="17" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="30"/>
-      <c r="B8" s="30"/>
-      <c r="C8" s="30"/>
+      <c r="A8" s="31"/>
+      <c r="B8" s="31"/>
+      <c r="C8" s="31"/>
       <c r="D8" s="17" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="30"/>
-      <c r="B9" s="30"/>
-      <c r="C9" s="30"/>
-      <c r="D9" s="17" t="s">
+      <c r="A9" s="31"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="25" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="30"/>
-      <c r="B10" s="30"/>
-      <c r="C10" s="30"/>
+      <c r="A10" s="31"/>
+      <c r="B10" s="31"/>
+      <c r="C10" s="31"/>
       <c r="D10" s="17" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="30"/>
-      <c r="B11" s="30"/>
-      <c r="C11" s="30"/>
+      <c r="A11" s="31"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="31"/>
       <c r="D11" s="17" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="30"/>
-      <c r="B12" s="30"/>
-      <c r="C12" s="30"/>
-      <c r="D12" s="17" t="s">
+      <c r="A12" s="31"/>
+      <c r="B12" s="31"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="25" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="30"/>
-      <c r="B13" s="30"/>
-      <c r="C13" s="30"/>
+      <c r="A13" s="31"/>
+      <c r="B13" s="31"/>
+      <c r="C13" s="31"/>
       <c r="D13" s="17" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="30"/>
-      <c r="B14" s="30"/>
-      <c r="C14" s="30"/>
+      <c r="A14" s="31"/>
+      <c r="B14" s="31"/>
+      <c r="C14" s="31"/>
       <c r="D14" s="17" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="30"/>
-      <c r="B15" s="30"/>
-      <c r="C15" s="30"/>
+      <c r="A15" s="31"/>
+      <c r="B15" s="31"/>
+      <c r="C15" s="31"/>
       <c r="D15" s="17" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" s="30"/>
-      <c r="B16" s="30"/>
-      <c r="C16" s="30"/>
-      <c r="D16" s="17" t="s">
+      <c r="A16" s="31"/>
+      <c r="B16" s="31"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="25" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" s="30" t="s">
+      <c r="A17" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="B17" s="30" t="s">
+      <c r="B17" s="31" t="s">
         <v>79</v>
       </c>
-      <c r="C17" s="30">
+      <c r="C17" s="31">
         <v>6</v>
       </c>
       <c r="D17" s="17" t="s">
@@ -1840,25 +2110,25 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A18" s="30"/>
-      <c r="B18" s="30"/>
-      <c r="C18" s="30"/>
+      <c r="A18" s="31"/>
+      <c r="B18" s="31"/>
+      <c r="C18" s="31"/>
       <c r="D18" s="17" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A19" s="30"/>
-      <c r="B19" s="30"/>
-      <c r="C19" s="30"/>
+      <c r="A19" s="31"/>
+      <c r="B19" s="31"/>
+      <c r="C19" s="31"/>
       <c r="D19" s="17" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A20" s="30"/>
-      <c r="B20" s="30"/>
-      <c r="C20" s="30"/>
+      <c r="A20" s="31"/>
+      <c r="B20" s="31"/>
+      <c r="C20" s="31"/>
       <c r="D20" s="17" t="s">
         <v>82</v>
       </c>
@@ -2140,4 +2410,347 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69F32D34-9A7B-0B4C-98E9-1B5068E60CA6}">
+  <dimension ref="A1:E19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="140.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="32" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" s="33" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="33" t="s">
+        <v>113</v>
+      </c>
+      <c r="D1" s="33" t="s">
+        <v>114</v>
+      </c>
+      <c r="E1" s="34" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="35" t="s">
+        <v>116</v>
+      </c>
+      <c r="B2" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="36" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" s="36">
+        <v>26</v>
+      </c>
+      <c r="E2" s="37" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="38" t="s">
+        <v>116</v>
+      </c>
+      <c r="B3" s="39" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="39" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" s="39">
+        <v>27</v>
+      </c>
+      <c r="E3" s="40" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A4" s="41" t="s">
+        <v>116</v>
+      </c>
+      <c r="B4" s="42" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" s="42" t="s">
+        <v>61</v>
+      </c>
+      <c r="D4" s="42">
+        <v>28</v>
+      </c>
+      <c r="E4" s="43" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="128" x14ac:dyDescent="0.2">
+      <c r="A5" s="38" t="s">
+        <v>116</v>
+      </c>
+      <c r="B5" s="39" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" s="39" t="s">
+        <v>98</v>
+      </c>
+      <c r="D5" s="39">
+        <v>47</v>
+      </c>
+      <c r="E5" s="44" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="128" x14ac:dyDescent="0.2">
+      <c r="A6" s="41" t="s">
+        <v>116</v>
+      </c>
+      <c r="B6" s="42" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="D6" s="42">
+        <v>48</v>
+      </c>
+      <c r="E6" s="45" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="38" t="s">
+        <v>116</v>
+      </c>
+      <c r="B7" s="39" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" s="39"/>
+      <c r="D7" s="39">
+        <v>49</v>
+      </c>
+      <c r="E7" s="44" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="41" t="s">
+        <v>116</v>
+      </c>
+      <c r="B8" s="42" t="s">
+        <v>66</v>
+      </c>
+      <c r="C8" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="D8" s="42">
+        <v>50</v>
+      </c>
+      <c r="E8" s="46" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="38" t="s">
+        <v>116</v>
+      </c>
+      <c r="B9" s="39" t="s">
+        <v>66</v>
+      </c>
+      <c r="C9" s="39" t="s">
+        <v>98</v>
+      </c>
+      <c r="D9" s="39">
+        <v>51</v>
+      </c>
+      <c r="E9" s="47" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="41" t="s">
+        <v>116</v>
+      </c>
+      <c r="B10" s="42" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="D10" s="42">
+        <v>52</v>
+      </c>
+      <c r="E10" s="46" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="38" t="s">
+        <v>116</v>
+      </c>
+      <c r="B11" s="39" t="s">
+        <v>85</v>
+      </c>
+      <c r="C11" s="39" t="s">
+        <v>86</v>
+      </c>
+      <c r="D11" s="39">
+        <v>29</v>
+      </c>
+      <c r="E11" s="44" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="41" t="s">
+        <v>116</v>
+      </c>
+      <c r="B12" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="C12" s="42" t="s">
+        <v>86</v>
+      </c>
+      <c r="D12" s="42">
+        <v>30</v>
+      </c>
+      <c r="E12" s="45" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A13" s="38" t="s">
+        <v>116</v>
+      </c>
+      <c r="B13" s="39" t="s">
+        <v>85</v>
+      </c>
+      <c r="C13" s="39" t="s">
+        <v>86</v>
+      </c>
+      <c r="D13" s="39">
+        <v>31</v>
+      </c>
+      <c r="E13" s="44" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="41" t="s">
+        <v>116</v>
+      </c>
+      <c r="B14" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="C14" s="42" t="s">
+        <v>86</v>
+      </c>
+      <c r="D14" s="42">
+        <v>32</v>
+      </c>
+      <c r="E14" s="45" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="38" t="s">
+        <v>116</v>
+      </c>
+      <c r="B15" s="39" t="s">
+        <v>95</v>
+      </c>
+      <c r="C15" s="39" t="s">
+        <v>128</v>
+      </c>
+      <c r="D15" s="39">
+        <v>33</v>
+      </c>
+      <c r="E15" s="44" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="41" t="s">
+        <v>116</v>
+      </c>
+      <c r="B16" s="42" t="s">
+        <v>95</v>
+      </c>
+      <c r="C16" s="42" t="s">
+        <v>128</v>
+      </c>
+      <c r="D16" s="42">
+        <v>34</v>
+      </c>
+      <c r="E16" s="48" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" s="38" t="s">
+        <v>116</v>
+      </c>
+      <c r="B17" s="39" t="s">
+        <v>102</v>
+      </c>
+      <c r="C17" s="39" t="s">
+        <v>103</v>
+      </c>
+      <c r="D17" s="39">
+        <v>35</v>
+      </c>
+      <c r="E17" s="44" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A18" s="41" t="s">
+        <v>116</v>
+      </c>
+      <c r="B18" s="42" t="s">
+        <v>102</v>
+      </c>
+      <c r="C18" s="42" t="s">
+        <v>103</v>
+      </c>
+      <c r="D18" s="42">
+        <v>36</v>
+      </c>
+      <c r="E18" s="45" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" s="38" t="s">
+        <v>116</v>
+      </c>
+      <c r="B19" s="39" t="s">
+        <v>102</v>
+      </c>
+      <c r="C19" s="39" t="s">
+        <v>103</v>
+      </c>
+      <c r="D19" s="39">
+        <v>37</v>
+      </c>
+      <c r="E19" s="44" t="s">
+        <v>133</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>